<commit_message>
Added ipython notebooks for documentation, updated tasklist
</commit_message>
<xml_diff>
--- a/organization/timeline.xlsx
+++ b/organization/timeline.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LeonhardS/Documents/CSE/GIT/CS109/flightbbq/organization/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>What?</t>
   </si>
@@ -556,9 +551,9 @@
   <cellStyles count="5">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -825,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -839,9 +834,9 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
@@ -897,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -956,7 +951,7 @@
         <v>42348</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="112">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -966,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -983,7 +978,7 @@
       </c>
       <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="B5" s="20" t="s">
         <v>35</v>
       </c>
@@ -996,7 +991,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
@@ -1016,6 +1011,11 @@
     <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1023,22 +1023,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="13" width="21.83203125" customWidth="1"/>
     <col min="15" max="15" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="19">
       <c r="B2" s="21" t="s">
         <v>15</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="L2" s="31"/>
       <c r="M2" s="32"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="128" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="128">
       <c r="B4" s="13" t="s">
         <v>20</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="80">
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="112">
       <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B7" s="13" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B8" s="13" t="s">
         <v>43</v>
       </c>
@@ -1267,12 +1267,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
+      <c r="B9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1297,12 +1299,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
+      <c r="B10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="10"/>
@@ -1319,7 +1323,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B11" s="10" t="s">
         <v>56</v>
       </c>
@@ -1337,7 +1341,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>58</v>
       </c>
@@ -1355,7 +1359,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1369,7 +1373,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1383,7 +1387,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1397,7 +1401,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1411,7 +1415,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1425,7 +1429,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1439,7 +1443,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1453,7 +1457,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1467,7 +1471,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1481,7 +1485,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1495,7 +1499,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1509,7 +1513,7 @@
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1523,7 +1527,7 @@
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1537,7 +1541,7 @@
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1551,7 +1555,7 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1565,7 +1569,7 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1579,7 +1583,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1593,7 +1597,7 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1607,7 +1611,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1621,7 +1625,7 @@
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1635,7 +1639,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1649,7 +1653,7 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1663,7 +1667,7 @@
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1677,7 +1681,7 @@
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1691,7 +1695,7 @@
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -1705,7 +1709,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -1719,7 +1723,7 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -1733,7 +1737,7 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1747,7 +1751,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -1761,7 +1765,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
     </row>
-    <row r="42" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -1775,7 +1779,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -1789,7 +1793,7 @@
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
     </row>
-    <row r="44" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -1803,7 +1807,7 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -1817,7 +1821,7 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
     </row>
-    <row r="46" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
@@ -1831,7 +1835,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
@@ -1845,7 +1849,7 @@
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
     </row>
-    <row r="48" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -1859,7 +1863,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
     </row>
-    <row r="49" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -1873,7 +1877,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
     </row>
-    <row r="50" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -1887,7 +1891,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
     </row>
-    <row r="51" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -1901,7 +1905,7 @@
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
     </row>
-    <row r="52" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1915,7 +1919,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -1929,7 +1933,7 @@
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -1943,7 +1947,7 @@
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
     </row>
-    <row r="55" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -1957,7 +1961,7 @@
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
     </row>
-    <row r="56" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -1971,7 +1975,7 @@
       <c r="L56" s="10"/>
       <c r="M56" s="10"/>
     </row>
-    <row r="57" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -1985,7 +1989,7 @@
       <c r="L57" s="10"/>
       <c r="M57" s="10"/>
     </row>
-    <row r="58" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -1999,7 +2003,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -2013,7 +2017,7 @@
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
     </row>
-    <row r="60" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -2027,7 +2031,7 @@
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
     </row>
-    <row r="61" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -2041,7 +2045,7 @@
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
     </row>
-    <row r="62" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -2055,7 +2059,7 @@
       <c r="L62" s="10"/>
       <c r="M62" s="10"/>
     </row>
-    <row r="63" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -2069,7 +2073,7 @@
       <c r="L63" s="10"/>
       <c r="M63" s="10"/>
     </row>
-    <row r="64" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -2083,7 +2087,7 @@
       <c r="L64" s="10"/>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -2097,7 +2101,7 @@
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -2111,7 +2115,7 @@
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -2125,7 +2129,7 @@
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
     </row>
-    <row r="68" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -2139,7 +2143,7 @@
       <c r="L68" s="10"/>
       <c r="M68" s="10"/>
     </row>
-    <row r="69" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -2153,7 +2157,7 @@
       <c r="L69" s="10"/>
       <c r="M69" s="10"/>
     </row>
-    <row r="70" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -2167,7 +2171,7 @@
       <c r="L70" s="10"/>
       <c r="M70" s="10"/>
     </row>
-    <row r="71" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
@@ -2181,7 +2185,7 @@
       <c r="L71" s="10"/>
       <c r="M71" s="10"/>
     </row>
-    <row r="72" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -2195,7 +2199,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -2209,7 +2213,7 @@
       <c r="L73" s="10"/>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -2223,7 +2227,7 @@
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -2237,7 +2241,7 @@
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" s="2" customFormat="1" ht="84" customHeight="1">
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -2251,7 +2255,7 @@
       <c r="L76" s="10"/>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13">
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -2265,7 +2269,7 @@
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13">
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -2279,7 +2283,7 @@
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13">
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -2293,7 +2297,7 @@
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13">
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -2307,7 +2311,7 @@
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:13">
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
@@ -2321,7 +2325,7 @@
       <c r="L81" s="11"/>
       <c r="M81" s="11"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:13">
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
@@ -2335,7 +2339,7 @@
       <c r="L82" s="11"/>
       <c r="M82" s="11"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:13">
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
@@ -2349,7 +2353,7 @@
       <c r="L83" s="11"/>
       <c r="M83" s="11"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:13">
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
@@ -2363,7 +2367,7 @@
       <c r="L84" s="11"/>
       <c r="M84" s="11"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:13">
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
@@ -2377,7 +2381,7 @@
       <c r="L85" s="11"/>
       <c r="M85" s="11"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:13">
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -2391,7 +2395,7 @@
       <c r="L86" s="11"/>
       <c r="M86" s="11"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:13">
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -2405,7 +2409,7 @@
       <c r="L87" s="11"/>
       <c r="M87" s="11"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:13">
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -2419,7 +2423,7 @@
       <c r="L88" s="11"/>
       <c r="M88" s="11"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:13">
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -2433,7 +2437,7 @@
       <c r="L89" s="11"/>
       <c r="M89" s="11"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:13">
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -2447,7 +2451,7 @@
       <c r="L90" s="11"/>
       <c r="M90" s="11"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:13">
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
@@ -2461,7 +2465,7 @@
       <c r="L91" s="11"/>
       <c r="M91" s="11"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:13">
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
@@ -2475,7 +2479,7 @@
       <c r="L92" s="11"/>
       <c r="M92" s="11"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:13">
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
@@ -2489,7 +2493,7 @@
       <c r="L93" s="11"/>
       <c r="M93" s="11"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:13">
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
@@ -2503,7 +2507,7 @@
       <c r="L94" s="11"/>
       <c r="M94" s="11"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:13">
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
@@ -2517,7 +2521,7 @@
       <c r="L95" s="11"/>
       <c r="M95" s="11"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:13">
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
@@ -2531,7 +2535,7 @@
       <c r="L96" s="11"/>
       <c r="M96" s="11"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13">
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
@@ -2545,7 +2549,7 @@
       <c r="L97" s="11"/>
       <c r="M97" s="11"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:13">
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
@@ -2559,7 +2563,7 @@
       <c r="L98" s="11"/>
       <c r="M98" s="11"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:13">
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
@@ -2573,7 +2577,7 @@
       <c r="L99" s="11"/>
       <c r="M99" s="11"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:13">
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
@@ -2587,7 +2591,7 @@
       <c r="L100" s="11"/>
       <c r="M100" s="11"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:13">
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
@@ -2601,7 +2605,7 @@
       <c r="L101" s="11"/>
       <c r="M101" s="11"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:13">
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
@@ -2615,7 +2619,7 @@
       <c r="L102" s="11"/>
       <c r="M102" s="11"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:13">
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
@@ -2629,7 +2633,7 @@
       <c r="L103" s="11"/>
       <c r="M103" s="11"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:13">
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
@@ -2643,7 +2647,7 @@
       <c r="L104" s="11"/>
       <c r="M104" s="11"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:13">
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
@@ -2657,7 +2661,7 @@
       <c r="L105" s="11"/>
       <c r="M105" s="11"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:13">
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -2671,7 +2675,7 @@
       <c r="L106" s="11"/>
       <c r="M106" s="11"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:13">
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -2685,7 +2689,7 @@
       <c r="L107" s="11"/>
       <c r="M107" s="11"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:13">
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -2699,7 +2703,7 @@
       <c r="L108" s="11"/>
       <c r="M108" s="11"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:13">
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
@@ -2713,7 +2717,7 @@
       <c r="L109" s="11"/>
       <c r="M109" s="11"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:13">
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -2727,7 +2731,7 @@
       <c r="L110" s="11"/>
       <c r="M110" s="11"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:13">
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
@@ -2741,7 +2745,7 @@
       <c r="L111" s="11"/>
       <c r="M111" s="11"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:13">
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
@@ -2755,7 +2759,7 @@
       <c r="L112" s="11"/>
       <c r="M112" s="11"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:13">
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
@@ -2769,7 +2773,7 @@
       <c r="L113" s="11"/>
       <c r="M113" s="11"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:13">
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
@@ -2783,7 +2787,7 @@
       <c r="L114" s="11"/>
       <c r="M114" s="11"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:13">
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
@@ -2797,7 +2801,7 @@
       <c r="L115" s="11"/>
       <c r="M115" s="11"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:13">
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -2820,5 +2824,10 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>